<commit_message>
feat: experiment chart updates; spelling fixes; sticking to ntu library format
Signed-off-by: Tom Huang <r06942065@ntu.edu.tw>
</commit_message>
<xml_diff>
--- a/img_src/plots.xlsx
+++ b/img_src/plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom6311tom6311/Desktop/ntu-thesis/img_src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70F8670-73E7-F843-99A4-9C9A49F1D0D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4961C0-96D6-414E-98B6-47F05B586979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" firstSheet="3" activeTab="14" xr2:uid="{E697E83A-201A-3E47-BD96-3119B5C03217}"/>
+    <workbookView xWindow="9780" yWindow="-19620" windowWidth="28800" windowHeight="16220" firstSheet="3" activeTab="14" xr2:uid="{E697E83A-201A-3E47-BD96-3119B5C03217}"/>
   </bookViews>
   <sheets>
     <sheet name="exp3" sheetId="1" r:id="rId1"/>
@@ -58,8 +58,30 @@
     <definedName name="_xlchart.v1.31" hidden="1">'exp6(II)'!$F$2:$F$62</definedName>
     <definedName name="_xlchart.v1.32" hidden="1">'exp6(II)'!$G$1</definedName>
     <definedName name="_xlchart.v1.33" hidden="1">'exp6(II)'!$G$2:$G$62</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'exp6(II)'!$B$2:$B$62</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'exp6(II)'!$C$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'exp6(II)'!$C$2:$C$62</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'exp6(II)'!$D$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'exp6(II)'!$D$2:$D$62</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'exp6(II)'!$E$1</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'exp7 (II)'!$E$3:$E$32</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'exp6(II)'!$E$2:$E$62</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'exp6(II)'!$F$1</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'exp6(II)'!$F$2:$F$62</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'exp6(II)'!$G$1</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'exp6(II)'!$G$2:$G$62</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'exp6(II)'!$B$2:$B$62</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">'exp6(II)'!$C$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">'exp6(II)'!$C$2:$C$62</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">'exp6(II)'!$D$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">'exp6(II)'!$D$2:$D$62</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'exp8'!$A$3:$A$62</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">'exp6(II)'!$E$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">'exp6(II)'!$E$2:$E$62</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">'exp6(II)'!$F$1</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">'exp6(II)'!$F$2:$F$62</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">'exp6(II)'!$G$1</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">'exp6(II)'!$G$2:$G$62</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'exp8'!$C$2</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'exp8'!$C$3:$C$62</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'exp8'!$D$2</definedName>
@@ -31120,8 +31142,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -31160,7 +31182,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="6496050" y="190500"/>
-              <a:ext cx="7753350" cy="3924300"/>
+              <a:ext cx="7753350" cy="5651500"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -37578,8 +37600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68141B65-4AC3-184D-B851-FD31148E4E98}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -38226,6 +38248,9 @@
       <c r="F27">
         <v>1.5297619047619</v>
       </c>
+      <c r="G27">
+        <v>1.37638888888888</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
@@ -38247,6 +38272,9 @@
       <c r="F28">
         <v>1.57369942196531</v>
       </c>
+      <c r="G28">
+        <v>1.39923469387755</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
@@ -38268,6 +38296,9 @@
       <c r="F29">
         <v>1.5833333333333299</v>
       </c>
+      <c r="G29">
+        <v>1.4736111111111101</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
@@ -38289,6 +38320,9 @@
       <c r="F30">
         <v>1.6286982248520701</v>
       </c>
+      <c r="G30">
+        <v>1.4820359281437101</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
@@ -38310,6 +38344,9 @@
       <c r="F31">
         <v>1.67628205128205</v>
       </c>
+      <c r="G31">
+        <v>1.45757575757575</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
@@ -38331,6 +38368,9 @@
       <c r="F32">
         <v>1.6982142857142799</v>
       </c>
+      <c r="G32">
+        <v>1.51515151515151</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
@@ -38340,6 +38380,21 @@
         <f>A33*10</f>
         <v>10</v>
       </c>
+      <c r="C33">
+        <v>1.5359477124183001</v>
+      </c>
+      <c r="D33">
+        <v>1.10248447204968</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
@@ -38349,6 +38404,21 @@
         <f t="shared" ref="B34:B47" si="2">A34*10</f>
         <v>20</v>
       </c>
+      <c r="C34">
+        <v>1.89619883040935</v>
+      </c>
+      <c r="D34">
+        <v>1.3859375</v>
+      </c>
+      <c r="E34">
+        <v>1.11057692307692</v>
+      </c>
+      <c r="F34">
+        <v>1.01687116564417</v>
+      </c>
+      <c r="G34">
+        <v>1.0014619883040901</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
@@ -38358,6 +38428,21 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
+      <c r="C35">
+        <v>2.27678571428571</v>
+      </c>
+      <c r="D35">
+        <v>1.5177419354838699</v>
+      </c>
+      <c r="E35">
+        <v>1.2439613526569999</v>
+      </c>
+      <c r="F35">
+        <v>1.1048951048950999</v>
+      </c>
+      <c r="G35">
+        <v>1.03266331658291</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
@@ -38367,6 +38452,21 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
+      <c r="C36">
+        <v>2.4455882352941098</v>
+      </c>
+      <c r="D36">
+        <v>1.76479289940828</v>
+      </c>
+      <c r="E36">
+        <v>1.3515625</v>
+      </c>
+      <c r="F36">
+        <v>1.1925465838509299</v>
+      </c>
+      <c r="G36">
+        <v>1.0796089385474801</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
@@ -38376,6 +38476,21 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
+      <c r="C37">
+        <v>2.6651234567901199</v>
+      </c>
+      <c r="D37">
+        <v>1.8068181818181801</v>
+      </c>
+      <c r="E37">
+        <v>1.4644970414201099</v>
+      </c>
+      <c r="F37">
+        <v>1.27139037433155</v>
+      </c>
+      <c r="G37">
+        <v>1.1451612903225801</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38">
@@ -38385,6 +38500,21 @@
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
+      <c r="C38">
+        <v>2.7362804878048701</v>
+      </c>
+      <c r="D38">
+        <v>1.9660493827160399</v>
+      </c>
+      <c r="E38">
+        <v>1.51344086021505</v>
+      </c>
+      <c r="F38">
+        <v>1.3371710526315701</v>
+      </c>
+      <c r="G38">
+        <v>1.19938650306748</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
@@ -38394,6 +38524,21 @@
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
+      <c r="C39">
+        <v>2.8026315789473601</v>
+      </c>
+      <c r="D39">
+        <v>2.0454545454545401</v>
+      </c>
+      <c r="E39">
+        <v>1.61728395061728</v>
+      </c>
+      <c r="F39">
+        <v>1.3801369863013699</v>
+      </c>
+      <c r="G39">
+        <v>1.20926966292134</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
@@ -38403,7 +38548,21 @@
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="C40">
+        <v>2.8159509202453901</v>
+      </c>
+      <c r="D40">
+        <v>2.14798850574712</v>
+      </c>
+      <c r="E40">
+        <v>1.64786585365853</v>
+      </c>
+      <c r="F40">
+        <v>1.4654696132596601</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1.2671232876712299</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
@@ -38413,6 +38572,21 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
+      <c r="C41">
+        <v>2.9401197604790399</v>
+      </c>
+      <c r="D41">
+        <v>2.2100591715976301</v>
+      </c>
+      <c r="E41">
+        <v>1.75552486187845</v>
+      </c>
+      <c r="F41">
+        <v>1.4787878787878701</v>
+      </c>
+      <c r="G41">
+        <v>1.3139204545454499</v>
+      </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
@@ -38422,6 +38596,21 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
+      <c r="C42">
+        <v>2.69504310344827</v>
+      </c>
+      <c r="D42">
+        <v>2.2361111111111098</v>
+      </c>
+      <c r="E42">
+        <v>1.8070652173913</v>
+      </c>
+      <c r="F42">
+        <v>1.5536723163841799</v>
+      </c>
+      <c r="G42">
+        <v>1.3884180790960401</v>
+      </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
@@ -38431,6 +38620,21 @@
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
+      <c r="C43">
+        <v>3.1722560975609699</v>
+      </c>
+      <c r="D43">
+        <v>2.29458598726114</v>
+      </c>
+      <c r="E43">
+        <v>1.8128140703517499</v>
+      </c>
+      <c r="F43">
+        <v>1.6150568181818099</v>
+      </c>
+      <c r="G43">
+        <v>1.3964497041420101</v>
+      </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
@@ -38440,6 +38644,21 @@
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
+      <c r="C44">
+        <v>3.2390109890109802</v>
+      </c>
+      <c r="D44">
+        <v>2.3294117647058799</v>
+      </c>
+      <c r="E44">
+        <v>1.8128415300546401</v>
+      </c>
+      <c r="F44">
+        <v>1.6298076923076901</v>
+      </c>
+      <c r="G44">
+        <v>1.4388586956521701</v>
+      </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
@@ -38449,6 +38668,21 @@
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
+      <c r="C45">
+        <v>3.24277456647398</v>
+      </c>
+      <c r="D45">
+        <v>2.3818181818181801</v>
+      </c>
+      <c r="E45">
+        <v>1.88636363636363</v>
+      </c>
+      <c r="F45">
+        <v>1.6640127388535</v>
+      </c>
+      <c r="G45">
+        <v>1.4799382716049301</v>
+      </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
@@ -38458,6 +38692,21 @@
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
+      <c r="C46">
+        <v>3.3963815789473601</v>
+      </c>
+      <c r="D46">
+        <v>2.41166666666666</v>
+      </c>
+      <c r="E46">
+        <v>1.9294478527607299</v>
+      </c>
+      <c r="F46">
+        <v>1.63102409638554</v>
+      </c>
+      <c r="G46">
+        <v>1.48479729729729</v>
+      </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
@@ -38467,6 +38716,21 @@
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
+      <c r="C47">
+        <v>3.32407407407407</v>
+      </c>
+      <c r="D47">
+        <v>2.4619205298013198</v>
+      </c>
+      <c r="E47">
+        <v>1.94785276073619</v>
+      </c>
+      <c r="F47">
+        <v>1.6781767955801099</v>
+      </c>
+      <c r="G47">
+        <v>1.51107594936708</v>
+      </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
@@ -38476,8 +38740,11 @@
         <f>A48*10</f>
         <v>10</v>
       </c>
+      <c r="C48">
+        <v>1.54905063291139</v>
+      </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -38485,8 +38752,11 @@
         <f t="shared" ref="B49:B62" si="3">A49*10</f>
         <v>20</v>
       </c>
+      <c r="C49">
+        <v>1.92901234567901</v>
+      </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>3</v>
       </c>
@@ -38494,8 +38764,11 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
+      <c r="C50">
+        <v>2.2105263157894699</v>
+      </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>4</v>
       </c>
@@ -38503,8 +38776,11 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
+      <c r="C51">
+        <v>2.3734375000000001</v>
+      </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -38512,8 +38788,11 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
+      <c r="C52">
+        <v>2.5968208092485501</v>
+      </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>6</v>
       </c>
@@ -38521,8 +38800,11 @@
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
+      <c r="C53">
+        <v>2.6694915254237199</v>
+      </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>7</v>
       </c>
@@ -38530,8 +38812,11 @@
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
+      <c r="C54">
+        <v>2.7704678362573101</v>
+      </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>8</v>
       </c>
@@ -38539,8 +38824,11 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
+      <c r="C55">
+        <v>2.87053571428571</v>
+      </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>9</v>
       </c>
@@ -38548,8 +38836,11 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
+      <c r="C56">
+        <v>2.92837078651685</v>
+      </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>10</v>
       </c>
@@ -38557,8 +38848,11 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
+      <c r="C57">
+        <v>3.0464480874316902</v>
+      </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>11</v>
       </c>
@@ -38566,8 +38860,11 @@
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
+      <c r="C58">
+        <v>3.1967455621301699</v>
+      </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>12</v>
       </c>
@@ -38575,8 +38872,11 @@
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
+      <c r="C59">
+        <v>3.2397959183673399</v>
+      </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>13</v>
       </c>
@@ -38584,8 +38884,11 @@
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
+      <c r="C60">
+        <v>3.2383040935672498</v>
+      </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>14</v>
       </c>
@@ -38593,14 +38896,20 @@
         <f t="shared" si="3"/>
         <v>140</v>
       </c>
+      <c r="C61">
+        <v>3.2515151515151501</v>
+      </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>15</v>
       </c>
       <c r="B62">
         <f t="shared" si="3"/>
         <v>150</v>
+      </c>
+      <c r="C62">
+        <v>3.36486486486486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>